<commit_message>
se realizan modificaiocnes en comparación subida excel al incluirlos en la app
</commit_message>
<xml_diff>
--- a/app/dataextraction/Recibos/Fechas_Clientes.xlsx
+++ b/app/dataextraction/Recibos/Fechas_Clientes.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazmin\Documents\Proyectos\proyecto-final-ekchy\app\dataextraction\Recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0B3164C-CD2B-4520-AFC4-38D266A8C02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C245A6-8941-41E3-80BF-76373772095F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes " sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
   <si>
     <t>pais</t>
   </si>
@@ -63,116 +62,95 @@
     <t>ARG</t>
   </si>
   <si>
+    <t>IVA</t>
+  </si>
+  <si>
+    <t>Juan Espinosa</t>
+  </si>
+  <si>
+    <t>30-70877589-0</t>
+  </si>
+  <si>
+    <t>IAFH GLOBAL SA</t>
+  </si>
+  <si>
+    <t>Camilo Sarmiento</t>
+  </si>
+  <si>
+    <t>30-69556267-1</t>
+  </si>
+  <si>
+    <t>DECISION SUPPORT SA</t>
+  </si>
+  <si>
+    <t>Flor Cardenas</t>
+  </si>
+  <si>
+    <t>30-71245283-4</t>
+  </si>
+  <si>
+    <t>DYNAFLOWS SA</t>
+  </si>
+  <si>
+    <t>Maria Rivera</t>
+  </si>
+  <si>
+    <t>30-70840691-7</t>
+  </si>
+  <si>
+    <t>SISTEMAS GLOBALES SA</t>
+  </si>
+  <si>
+    <t>COL</t>
+  </si>
+  <si>
+    <t>MEX</t>
+  </si>
+  <si>
+    <t>NPI620328DP8</t>
+  </si>
+  <si>
+    <t>NCS PEARSON, INC.</t>
+  </si>
+  <si>
+    <t>IVA DIGITALES</t>
+  </si>
+  <si>
+    <t>30-71509409-2</t>
+  </si>
+  <si>
+    <t>AMDIPHARM LTD</t>
+  </si>
+  <si>
+    <t>VIMEO.COM, INC.</t>
+  </si>
+  <si>
+    <t>GLOBANT COLOMBIA S.A.S</t>
+  </si>
+  <si>
     <t>30-70892838-7</t>
   </si>
   <si>
     <t>BSF SA</t>
   </si>
   <si>
-    <t>IVA</t>
-  </si>
-  <si>
-    <t>Juan Espinosa</t>
-  </si>
-  <si>
-    <t>30-70877589-0</t>
-  </si>
-  <si>
-    <t>IAFH GLOBAL SA</t>
-  </si>
-  <si>
-    <t>Camilo Sarmiento</t>
-  </si>
-  <si>
-    <t>30-69556267-1</t>
-  </si>
-  <si>
-    <t>DECISION SUPPORT SA</t>
-  </si>
-  <si>
-    <t>Flor Cardenas</t>
-  </si>
-  <si>
-    <t>30-71245283-4</t>
-  </si>
-  <si>
-    <t>DYNAFLOWS SA</t>
-  </si>
-  <si>
-    <t>Maria Rivera</t>
-  </si>
-  <si>
-    <t>30-70840691-7</t>
-  </si>
-  <si>
-    <t>SISTEMAS GLOBALES SA</t>
-  </si>
-  <si>
-    <t>COL</t>
-  </si>
-  <si>
     <t>900218578-7</t>
   </si>
   <si>
     <t>SISTEMAS COLOMBIA S.A.S</t>
   </si>
   <si>
-    <t>MEX</t>
-  </si>
-  <si>
-    <t>NPI620328DP8</t>
-  </si>
-  <si>
-    <t>NCS PEARSON, INC.</t>
-  </si>
-  <si>
-    <t>IVA DIGITALES</t>
-  </si>
-  <si>
-    <t>30-71509409-2</t>
-  </si>
-  <si>
-    <t>AMDIPHARM LTD</t>
-  </si>
-  <si>
     <t>AIRBNB IRELAND UNLIMITED COMPANY</t>
   </si>
   <si>
-    <t>VIMEO.COM, INC.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 901411533-6</t>
-  </si>
-  <si>
-    <t>GLOBANT COLOMBIA S.A.S</t>
-  </si>
-  <si>
-    <t>año</t>
-  </si>
-  <si>
-    <t>numeroFormulario</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> n_verificacion</t>
-  </si>
-  <si>
-    <t>saldoPagado</t>
-  </si>
-  <si>
-    <t>saldoFavor</t>
-  </si>
-  <si>
-    <t>Nombre Impuesto</t>
-  </si>
-  <si>
-    <t>fecha_procesado</t>
+    <t>901411533-6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -189,13 +167,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF24292F"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri Light"/>
@@ -210,18 +181,12 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -236,25 +201,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,47 +532,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20.109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="31.77734375" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -619,422 +580,348 @@
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
+      <c r="B2" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" s="3">
         <v>44631</v>
       </c>
       <c r="G2" s="3">
-        <f>+F2-3</f>
         <v>44628</v>
       </c>
       <c r="H2" s="3">
-        <f t="shared" ref="H2:H13" si="0">+G2-1</f>
         <v>44627</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
+      <c r="B3" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D3">
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" s="3">
         <v>44635</v>
       </c>
       <c r="G3" s="3">
-        <f>+F3-3</f>
         <v>44632</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" si="0"/>
         <v>44631</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
+      <c r="B4" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3">
         <v>44629</v>
       </c>
       <c r="G4" s="3">
-        <f>+F4-3</f>
         <v>44626</v>
       </c>
       <c r="H4" s="3">
-        <f t="shared" si="0"/>
         <v>44625</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
+      <c r="B5" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5">
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" s="3">
         <v>44635</v>
       </c>
       <c r="G5" s="3">
-        <f>+F5-1</f>
         <v>44634</v>
       </c>
       <c r="H5" s="3">
-        <f t="shared" si="0"/>
         <v>44633</v>
       </c>
       <c r="I5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>11</v>
+      <c r="B6" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="D6">
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6" s="3">
         <v>44630</v>
       </c>
       <c r="G6" s="3">
-        <f>+F6-3</f>
         <v>44627</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" si="0"/>
         <v>44626</v>
       </c>
       <c r="I6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7" s="3">
         <v>44636</v>
       </c>
       <c r="G7" s="3">
-        <f>+F7-3</f>
         <v>44633</v>
       </c>
       <c r="H7" s="3">
-        <f t="shared" si="0"/>
         <v>44632</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
+        <v>23</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" s="3">
         <v>44635</v>
       </c>
       <c r="G8" s="3">
-        <f>+F8-2</f>
         <v>44633</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" si="0"/>
         <v>44632</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
+        <v>24</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9">
-        <v>2</v>
-      </c>
-      <c r="E9" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="F9" s="3">
         <v>44639</v>
       </c>
       <c r="G9" s="3">
-        <f>+F9-2</f>
         <v>44637</v>
       </c>
       <c r="H9" s="3">
-        <f t="shared" si="0"/>
         <v>44636</v>
       </c>
-      <c r="I9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="I9" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="F10" s="3">
         <v>44637</v>
       </c>
       <c r="G10" s="3">
-        <f>+F10-3</f>
         <v>44634</v>
       </c>
       <c r="H10" s="3">
-        <f t="shared" si="0"/>
         <v>44633</v>
       </c>
-      <c r="I10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11">
+        <v>23</v>
+      </c>
+      <c r="B11" s="7">
         <v>9013543905</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="6">
+        <v>2</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="F11" s="3">
         <v>44639</v>
       </c>
       <c r="G11" s="3">
-        <f>+F11-3</f>
         <v>44636</v>
       </c>
       <c r="H11" s="3">
-        <f t="shared" si="0"/>
         <v>44635</v>
       </c>
-      <c r="I11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I11" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12">
+        <v>23</v>
+      </c>
+      <c r="B12" s="7">
         <v>901316197</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12" t="s">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="D12" s="6">
+        <v>2</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="F12" s="3">
         <v>44632</v>
       </c>
       <c r="G12" s="3">
-        <f>+F12-3</f>
         <v>44629</v>
       </c>
       <c r="H12" s="3">
-        <f t="shared" si="0"/>
         <v>44628</v>
       </c>
-      <c r="I12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
+        <v>31</v>
+      </c>
+      <c r="D13" s="6">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="F13" s="3">
         <v>44635</v>
       </c>
       <c r="G13" s="3">
-        <f>+F13-3</f>
         <v>44632</v>
       </c>
       <c r="H13" s="3">
-        <f t="shared" si="0"/>
         <v>44631</v>
       </c>
-      <c r="I13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EE8164-38C8-48E6-89D8-D70118D5227A}">
-  <dimension ref="A1:K1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:11" ht="16.8" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>44</v>
+      <c r="I13" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se realiza arreglo en funcion comparación y validación de datos al momento de cambiar proeso de documentos a procesado y no procesado, se crea una lista
</commit_message>
<xml_diff>
--- a/app/dataextraction/Recibos/Fechas_Clientes.xlsx
+++ b/app/dataextraction/Recibos/Fechas_Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazmin\Documents\Proyectos\proyecto-final-ekchy\app\dataextraction\Recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C245A6-8941-41E3-80BF-76373772095F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354E6FBF-E324-44FA-94C4-CE77172169C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
   <si>
     <t>pais</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>901411533-6</t>
+  </si>
+  <si>
+    <t>30-70892538-7</t>
+  </si>
+  <si>
+    <t>CONDOMINIO SIL FBSF SA</t>
   </si>
 </sst>
 </file>
@@ -220,7 +226,38 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -532,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD26"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,10 +734,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -925,6 +962,12 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
no duplicar excel id cronograma subidos en excel
</commit_message>
<xml_diff>
--- a/app/dataextraction/Recibos/Fechas_Clientes.xlsx
+++ b/app/dataextraction/Recibos/Fechas_Clientes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazmin\Documents\Proyectos\proyecto-final-ekchy\app\dataextraction\Recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354E6FBF-E324-44FA-94C4-CE77172169C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7DA0DB-089E-4110-B1D5-F286DC49D05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes " sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
   <si>
     <t>pais</t>
   </si>
@@ -116,18 +117,6 @@
     <t>IVA DIGITALES</t>
   </si>
   <si>
-    <t>30-71509409-2</t>
-  </si>
-  <si>
-    <t>AMDIPHARM LTD</t>
-  </si>
-  <si>
-    <t>VIMEO.COM, INC.</t>
-  </si>
-  <si>
-    <t>GLOBANT COLOMBIA S.A.S</t>
-  </si>
-  <si>
     <t>30-70892838-7</t>
   </si>
   <si>
@@ -138,12 +127,6 @@
   </si>
   <si>
     <t>SISTEMAS COLOMBIA S.A.S</t>
-  </si>
-  <si>
-    <t>AIRBNB IRELAND UNLIMITED COMPANY</t>
-  </si>
-  <si>
-    <t>901411533-6</t>
   </si>
   <si>
     <t>30-70892538-7</t>
@@ -226,7 +209,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -234,16 +217,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -567,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -618,10 +591,10 @@
         <v>9</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -734,10 +707,10 @@
         <v>9</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -792,10 +765,10 @@
         <v>23</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -845,129 +818,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="3">
-        <v>44637</v>
-      </c>
-      <c r="G10" s="3">
-        <v>44634</v>
-      </c>
-      <c r="H10" s="3">
-        <v>44633</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" s="7">
-        <v>9013543905</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="6">
-        <v>2</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3">
-        <v>44639</v>
-      </c>
-      <c r="G11" s="3">
-        <v>44636</v>
-      </c>
-      <c r="H11" s="3">
-        <v>44635</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="7">
-        <v>901316197</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="6">
-        <v>2</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="3">
-        <v>44632</v>
-      </c>
-      <c r="G12" s="3">
-        <v>44629</v>
-      </c>
-      <c r="H12" s="3">
-        <v>44628</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="6">
-        <v>2</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="3">
-        <v>44635</v>
-      </c>
-      <c r="G13" s="3">
-        <v>44632</v>
-      </c>
-      <c r="H13" s="3">
-        <v>44631</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+  <conditionalFormatting sqref="B1:B9">
+    <cfRule type="duplicateValues" dxfId="1" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="C1:C9">
+    <cfRule type="duplicateValues" dxfId="0" priority="12"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2794DDF7-E52E-49F9-9FCA-827870446694}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se realiza modificaciones de subida vencimientos meses anteriores
</commit_message>
<xml_diff>
--- a/app/dataextraction/Recibos/Fechas_Clientes.xlsx
+++ b/app/dataextraction/Recibos/Fechas_Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazmin\Documents\Proyectos\proyecto-final-ekchy\app\dataextraction\Recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7DA0DB-089E-4110-B1D5-F286DC49D05A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D708E835-33CB-4168-B7AC-88A1DBC51904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
se realiza cambios de decisiones y pasos a seguir
</commit_message>
<xml_diff>
--- a/app/dataextraction/Recibos/Fechas_Clientes.xlsx
+++ b/app/dataextraction/Recibos/Fechas_Clientes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jazmin\Documents\Proyectos\proyecto-final-ekchy\app\dataextraction\Recibos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D708E835-33CB-4168-B7AC-88A1DBC51904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81510DC7-F484-4227-925F-0A7ED7716BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>